<commit_message>
Initial on new computer
Initial on new computer
</commit_message>
<xml_diff>
--- a/result/GCM_Chol结果分析.xlsx
+++ b/result/GCM_Chol结果分析.xlsx
@@ -4,17 +4,18 @@
   <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010"/>
+    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="1000sign_7g" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="152511"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4" uniqueCount="4">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="50" uniqueCount="50">
   <si>
     <t>Cholesky_dim334Chol_CTskp_allFrame_370sign_Daily</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -28,6 +29,151 @@
   </si>
   <si>
     <t>GCM_658_10_allFrame_370sign_5g</t>
+  </si>
+  <si>
+    <t>Training time (s, 1000sign_6g): 3407.634936</t>
+  </si>
+  <si>
+    <t>Test time (s, 1000sign_1g): 694.516603</t>
+  </si>
+  <si>
+    <t>Training time (s, 1000sign_6g): 3420.985622</t>
+  </si>
+  <si>
+    <t>Test time (s, 1000sign_1g): 680.605085</t>
+  </si>
+  <si>
+    <t>Training time (s, 1000sign_6g): 3339.251506</t>
+  </si>
+  <si>
+    <t>Test time (s, 1000sign_1g): 691.708294</t>
+  </si>
+  <si>
+    <t>Training time (s, 1000sign_6g): 3384.821559</t>
+  </si>
+  <si>
+    <t>Test time (s, 1000sign_1g): 677.232352</t>
+  </si>
+  <si>
+    <t>Training time (s, 1000sign_6g): 3479.229588</t>
+  </si>
+  <si>
+    <t>Test time (s, 1000sign_1g): 694.526089</t>
+  </si>
+  <si>
+    <t>Training time (s, 1000sign_6g): 3345.614345</t>
+  </si>
+  <si>
+    <t>Test time (s, 1000sign_1g): 659.191073</t>
+  </si>
+  <si>
+    <t>Training time (s, 1000sign_6g): 3346.626920</t>
+  </si>
+  <si>
+    <t>Test time (s, 1000sign_1g): 683.032218</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Cov generation time cost (s, 1000sign_7g): 3468.642087 </t>
+  </si>
+  <si>
+    <t>GCM_658_10_allFrame_1000sign_7g</t>
+  </si>
+  <si>
+    <t>P10</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>P11</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>P14</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>P15</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>P17</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>P19</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>P21</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>P01</t>
+  </si>
+  <si>
+    <t>Training time (s, 1000sign_6g): 4953.295540</t>
+  </si>
+  <si>
+    <t>Test time (s, 1000sign_1g): 925.703454</t>
+  </si>
+  <si>
+    <t>P02</t>
+  </si>
+  <si>
+    <t>Training time (s, 1000sign_6g): 4925.330756</t>
+  </si>
+  <si>
+    <t>Test time (s, 1000sign_1g): 945.032503</t>
+  </si>
+  <si>
+    <t>P03</t>
+  </si>
+  <si>
+    <t>Training time (s, 1000sign_6g): 4999.542020</t>
+  </si>
+  <si>
+    <t>Test time (s, 1000sign_1g): 957.889348</t>
+  </si>
+  <si>
+    <t>P04</t>
+  </si>
+  <si>
+    <t>Training time (s, 1000sign_6g): 5085.707816</t>
+  </si>
+  <si>
+    <t>Test time (s, 1000sign_1g): 950.723484</t>
+  </si>
+  <si>
+    <t>P05</t>
+  </si>
+  <si>
+    <t>Training time (s, 1000sign_6g): 4685.187175</t>
+  </si>
+  <si>
+    <t>Test time (s, 1000sign_1g): 850.453575</t>
+  </si>
+  <si>
+    <t>P06</t>
+  </si>
+  <si>
+    <t>Training time (s, 1000sign_6g): 4820.550867</t>
+  </si>
+  <si>
+    <t>Test time (s, 1000sign_1g): 849.144249</t>
+  </si>
+  <si>
+    <t>P07</t>
+  </si>
+  <si>
+    <t>Training time (s, 1000sign_6g): 4573.051475</t>
+  </si>
+  <si>
+    <t>Test time (s, 1000sign_1g): 860.364045</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Cov generation time cost (s, 1000sign_7g): 3345.593645 </t>
+  </si>
+  <si>
+    <t>GCM_658_15_allFrame_1000sign_7g</t>
   </si>
 </sst>
 </file>
@@ -388,7 +534,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F19"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="C17" sqref="C17"/>
     </sheetView>
   </sheetViews>
@@ -548,4 +694,252 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="1200" verticalDpi="1200" r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:D22"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C20" sqref="C20"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>
+  <cols>
+    <col min="2" max="2" width="7" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:4" x14ac:dyDescent="0.15">
+      <c r="A1" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.15">
+      <c r="A2" t="s">
+        <v>20</v>
+      </c>
+      <c r="B2">
+        <v>76.900000000000006</v>
+      </c>
+      <c r="C2" t="s">
+        <v>4</v>
+      </c>
+      <c r="D2" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.15">
+      <c r="A3" t="s">
+        <v>21</v>
+      </c>
+      <c r="B3">
+        <v>79.900000000000006</v>
+      </c>
+      <c r="C3" t="s">
+        <v>6</v>
+      </c>
+      <c r="D3" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.15">
+      <c r="A4" t="s">
+        <v>22</v>
+      </c>
+      <c r="B4">
+        <v>77.3</v>
+      </c>
+      <c r="C4" t="s">
+        <v>8</v>
+      </c>
+      <c r="D4" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.15">
+      <c r="A5" t="s">
+        <v>23</v>
+      </c>
+      <c r="B5">
+        <v>78.900000000000006</v>
+      </c>
+      <c r="C5" t="s">
+        <v>10</v>
+      </c>
+      <c r="D5" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.15">
+      <c r="A6" t="s">
+        <v>24</v>
+      </c>
+      <c r="B6">
+        <v>74</v>
+      </c>
+      <c r="C6" t="s">
+        <v>12</v>
+      </c>
+      <c r="D6" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" x14ac:dyDescent="0.15">
+      <c r="A7" t="s">
+        <v>25</v>
+      </c>
+      <c r="B7">
+        <v>81</v>
+      </c>
+      <c r="C7" t="s">
+        <v>14</v>
+      </c>
+      <c r="D7" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4" x14ac:dyDescent="0.15">
+      <c r="A8" t="s">
+        <v>26</v>
+      </c>
+      <c r="B8">
+        <v>58.6</v>
+      </c>
+      <c r="C8" t="s">
+        <v>16</v>
+      </c>
+      <c r="D8" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4" x14ac:dyDescent="0.15">
+      <c r="B9" s="1">
+        <f>AVERAGE(B2:B8)</f>
+        <v>75.228571428571428</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4" x14ac:dyDescent="0.15">
+      <c r="A10" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="13" spans="1:4" x14ac:dyDescent="0.15">
+      <c r="A13" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="14" spans="1:4" x14ac:dyDescent="0.15">
+      <c r="A14" t="s">
+        <v>27</v>
+      </c>
+      <c r="B14">
+        <v>77.400000000000006</v>
+      </c>
+      <c r="C14" t="s">
+        <v>28</v>
+      </c>
+      <c r="D14" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="15" spans="1:4" x14ac:dyDescent="0.15">
+      <c r="A15" t="s">
+        <v>30</v>
+      </c>
+      <c r="B15">
+        <v>78.099999999999994</v>
+      </c>
+      <c r="C15" t="s">
+        <v>31</v>
+      </c>
+      <c r="D15" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="16" spans="1:4" x14ac:dyDescent="0.15">
+      <c r="A16" t="s">
+        <v>33</v>
+      </c>
+      <c r="B16">
+        <v>77</v>
+      </c>
+      <c r="C16" t="s">
+        <v>34</v>
+      </c>
+      <c r="D16" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="17" spans="1:4" x14ac:dyDescent="0.15">
+      <c r="A17" t="s">
+        <v>36</v>
+      </c>
+      <c r="B17">
+        <v>76.099999999999994</v>
+      </c>
+      <c r="C17" t="s">
+        <v>37</v>
+      </c>
+      <c r="D17" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="18" spans="1:4" x14ac:dyDescent="0.15">
+      <c r="A18" t="s">
+        <v>39</v>
+      </c>
+      <c r="B18">
+        <v>72.3</v>
+      </c>
+      <c r="C18" t="s">
+        <v>40</v>
+      </c>
+      <c r="D18" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="19" spans="1:4" x14ac:dyDescent="0.15">
+      <c r="A19" t="s">
+        <v>42</v>
+      </c>
+      <c r="B19">
+        <v>79.8</v>
+      </c>
+      <c r="C19" t="s">
+        <v>43</v>
+      </c>
+      <c r="D19" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="20" spans="1:4" x14ac:dyDescent="0.15">
+      <c r="A20" t="s">
+        <v>45</v>
+      </c>
+      <c r="B20">
+        <v>60.8</v>
+      </c>
+      <c r="C20" t="s">
+        <v>46</v>
+      </c>
+      <c r="D20" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="21" spans="1:4" x14ac:dyDescent="0.15">
+      <c r="B21" s="1">
+        <f>AVERAGE(B14:B20)</f>
+        <v>74.5</v>
+      </c>
+    </row>
+    <row r="22" spans="1:4" x14ac:dyDescent="0.15">
+      <c r="A22" t="s">
+        <v>48</v>
+      </c>
+    </row>
+  </sheetData>
+  <phoneticPr fontId="1" type="noConversion"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="1200" verticalDpi="1200" r:id="rId1"/>
+</worksheet>
 </file>
</xml_diff>